<commit_message>
-"Delete All" button now reloads the page. 	-It's now a form -> input button that sends request to /delete_all
</commit_message>
<xml_diff>
--- a/instance/generatedoutput.xlsx
+++ b/instance/generatedoutput.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,25 +451,140 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>joe dude corp</t>
+          <t>Super Corporation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>joe schmoe</t>
+          <t>Alex Reams</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>jschmore@gmail.com</t>
+          <t>areams@supercorp.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>555-555-1234</t>
+          <t>630-555-1234</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Helios Realty</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Emil Jones</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ejones@email.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>645-555-9630</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Super Corporation</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Alex Reams</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>areams@supercorp.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>630-555-1234</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Helios Realty</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Emil Jones</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ejones@email.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>645-555-9630</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Super Corporation</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Alex Reams</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>areams@supercorp.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>630-555-1234</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Helios Realty</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Emil Jones</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ejones@email.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>645-555-9630</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
-Implemented functionality of "delete-selected" button 	-checks the COMPANY NAMES of the selected rows and creates new session omitting those objects
-extra flask function "/echo" added for debugging; it echoes the request message it receives.
</commit_message>
<xml_diff>
--- a/instance/generatedoutput.xlsx
+++ b/instance/generatedoutput.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,22 +451,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Super Corporation</t>
+          <t>Example Corporation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alex Reams</t>
+          <t>Firstname Lastname</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>areams@supercorp.com</t>
+          <t>flastname@examplecorp.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>630-555-1234</t>
+          <t>123-555-1234</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -474,22 +474,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Helios Realty</t>
+          <t>Builder Co.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Emil Jones</t>
+          <t>Another Name</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ejones@email.com</t>
+          <t>aname@builderco.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>645-555-9630</t>
+          <t>321-555-4321</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -497,22 +497,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Super Corporation</t>
+          <t>Example Corporation</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Alex Reams</t>
+          <t>Firstname Lastname</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>areams@supercorp.com</t>
+          <t>flastname@examplecorp.com</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>630-555-1234</t>
+          <t>123-555-1234</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -520,71 +520,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Helios Realty</t>
+          <t>Builder Co.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Emil Jones</t>
+          <t>Another Name</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ejones@email.com</t>
+          <t>aname@builderco.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>645-555-9630</t>
+          <t>321-555-4321</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Super Corporation</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Alex Reams</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>areams@supercorp.com</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>630-555-1234</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Helios Realty</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Emil Jones</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>ejones@email.com</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>645-555-9630</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
began adding database to replace reliance on session
-will be using postgresql
	-began adding models.py
-added config.py to handle different sets of env vars
</commit_message>
<xml_diff>
--- a/instance/generatedoutput.xlsx
+++ b/instance/generatedoutput.xlsx
@@ -469,7 +469,11 @@
           <t>123-555-1234</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>3200 Progress Ln Eureka, CA 92000</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -489,7 +493,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>321-555-4321</t>
+          <t>(321) 555-4321</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -515,7 +519,11 @@
           <t>123-555-1234</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>3200 Progress Ln Eureka, CA 92000</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,7 +543,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>321-555-4321</t>
+          <t>(321) 555-4321</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>

</xml_diff>